<commit_message>
add another sample test case. update key for expected results
</commit_message>
<xml_diff>
--- a/export_key.xlsx
+++ b/export_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\pythonstuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\pythonstuff\avg_salary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB24332-1C70-447F-B06C-03BBAE8090FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70862D6F-6148-4298-B5E0-9F2C20F1AE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DED730B-9C02-4BD4-B0BC-8F6D78754AB7}"/>
+    <workbookView xWindow="60" yWindow="600" windowWidth="28740" windowHeight="15600" xr2:uid="{9DED730B-9C02-4BD4-B0BC-8F6D78754AB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>CSV TITLE</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>04/2017 - 03/2022</t>
+  </si>
+  <si>
+    <t>export_format9_quarters</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>07/2017 - 06/2022</t>
   </si>
 </sst>
 </file>
@@ -492,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D0859D-7E2A-404A-A6D1-838743F18A8E}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,29 +703,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>3958.91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B11:E12"/>
+    <mergeCell ref="B12:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>